<commit_message>
July 16- Added Ansible Roles header
</commit_message>
<xml_diff>
--- a/Devops Commands.xlsx
+++ b/Devops Commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevOps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CE53F6-E7D6-4C40-B85C-0E0052922CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133CF3ED-3AF6-465B-B3CC-881EABCA21D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{17903FFA-095F-4719-859A-9B63398CF432}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="258">
   <si>
     <t>ls</t>
   </si>
@@ -2275,6 +2275,9 @@
       </rPr>
       <t xml:space="preserve">  &gt;&gt;  [Lists of tasks to be performed]</t>
     </r>
+  </si>
+  <si>
+    <t>Ansible Roles</t>
   </si>
 </sst>
 </file>
@@ -2757,6 +2760,21 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2772,23 +2790,8 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4463,7 +4466,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DF488BB-F33B-465B-9A85-E4575B1FF101}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
@@ -4477,21 +4480,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:13" s="31" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="53" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="30"/>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -4578,11 +4581,11 @@
       <c r="B10" s="28"/>
     </row>
     <row r="11" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="54" t="s">
         <v>223</v>
       </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="33" t="s">
@@ -4638,11 +4641,11 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="45" t="s">
         <v>237</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="52"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
       <c r="M17" t="s">
         <v>197</v>
       </c>
@@ -4717,45 +4720,53 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="50" t="s">
+      <c r="A26" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="52"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47"/>
       <c r="M26" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="55" t="s">
         <v>235</v>
       </c>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
     </row>
     <row r="28" spans="1:13" ht="72.400000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>236</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="46"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
     </row>
     <row r="30" spans="1:13" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="45" t="s">
         <v>255</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="52"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="47"/>
     </row>
     <row r="31" spans="1:13" ht="146.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="48" t="s">
         <v>256</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+    </row>
+    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A33:C33"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A28:C28"/>

</xml_diff>